<commit_message>
Cài đặt NodeJS trên WSL tạo ứng dụng ExpressJS
</commit_message>
<xml_diff>
--- a/gioi-thieu-va-cai-dat-wsl-tren-windows/gioi-thieu-va-cai-dat-wsl-tren-windows.xlsx
+++ b/gioi-thieu-va-cai-dat-wsl-tren-windows/gioi-thieu-va-cai-dat-wsl-tren-windows.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\wsl\gioi-thieu-va-cai-dat-wsl-tren-windows\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDDA2D71-8D7D-4072-BF8C-4D9B13799535}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{866DBD23-21D0-4FCB-A722-A3C8935D2F12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Giới thiệu WSL" sheetId="1" r:id="rId1"/>
@@ -700,50 +700,6 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>96</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>561143</xdr:colOff>
-      <xdr:row>102</xdr:row>
-      <xdr:rowOff>114143</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="9" name="Picture 8">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CDD65D11-41D1-4119-AF57-E9F8A3674161}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="609600" y="18288000"/>
-          <a:ext cx="6657143" cy="1257143"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
       <xdr:row>106</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
@@ -767,7 +723,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -811,7 +767,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -855,7 +811,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -899,7 +855,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -943,7 +899,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -987,7 +943,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1031,7 +987,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1075,7 +1031,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1119,7 +1075,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1163,7 +1119,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1207,7 +1163,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1251,7 +1207,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1260,6 +1216,50 @@
         <a:xfrm>
           <a:off x="609600" y="73152000"/>
           <a:ext cx="6047619" cy="1323810"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>96</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>103</xdr:row>
+      <xdr:rowOff>56243</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E23D6EE0-4293-485A-95C4-1301967EAE4E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="18288000"/>
+          <a:ext cx="7296150" cy="1389743"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2090,7 +2090,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A05E9AD3-5BBD-4F45-B06D-229FBFECB250}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A73" workbookViewId="0">
       <selection activeCell="B92" sqref="B92"/>
     </sheetView>
   </sheetViews>
@@ -2105,8 +2105,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00AF2D5A-A670-4E11-9FD1-EB1362CE765B}">
   <dimension ref="A2:O384"/>
   <sheetViews>
-    <sheetView topLeftCell="A382" workbookViewId="0">
-      <selection activeCell="A394" sqref="A394"/>
+    <sheetView topLeftCell="A373" workbookViewId="0">
+      <selection activeCell="B348" sqref="B348"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2241,7 +2241,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C3EF4C3-46E8-4BD5-A2BF-F8FFD8467BC4}">
   <dimension ref="A2:B231"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A174" workbookViewId="0">
+    <sheetView topLeftCell="A174" workbookViewId="0">
       <selection activeCell="Q185" sqref="Q185"/>
     </sheetView>
   </sheetViews>
@@ -2327,7 +2327,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F638B4C-EA38-4D48-9481-E0B2AA185F2F}">
   <dimension ref="A2:B23"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>

</xml_diff>